<commit_message>
Complete Automation of NewTours Site
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="excelflightfind" sheetId="2" r:id="rId2"/>
+    <sheet name="excelbookflight" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>demo</t>
   </si>
@@ -29,6 +30,30 @@
   </si>
   <si>
     <t>Paris</t>
+  </si>
+  <si>
+    <t>Imran</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Tasrifa</t>
+  </si>
+  <si>
+    <t>Pomy</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Aiub</t>
+  </si>
+  <si>
+    <t>Adabor</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
   </si>
 </sst>
 </file>
@@ -371,7 +396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -403,4 +428,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1">
+        <v>123456789</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1">
+        <v>1207</v>
+      </c>
+      <c r="N1">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>